<commit_message>
Process Raw function working.
</commit_message>
<xml_diff>
--- a/test2.xlsx
+++ b/test2.xlsx
@@ -124,10 +124,10 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¯ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¼ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ­ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¯ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¼ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ³ ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¯ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¼ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ°ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ£ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ´ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ£ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ·ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ£ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ£ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¯"/>
-        <a:font script="Hang" typeface="ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ«ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ§ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¬ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂªÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ³ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ«ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ"/>
-        <a:font script="Hans" typeface="ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¥ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ®ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¤ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ½ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ"/>
-        <a:font script="Hant" typeface="ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¦ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ°ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ§ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ´ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ°ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¦ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ©ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ«ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ"/>
+        <a:font script="Jpan" typeface="ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¯ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¼ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ­ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¯ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¼ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ³ ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¯ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¼ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ°ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ£ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ´ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ£ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ·ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ£ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ£ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¯"/>
+        <a:font script="Hang" typeface="ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ«ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ§ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¬ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂªÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ³ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ«ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ"/>
+        <a:font script="Hans" typeface="ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¥ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ®ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¤ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ½ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ"/>
+        <a:font script="Hant" typeface="ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¦ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ°ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ§ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ´ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ°ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¦ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ©ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ«ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
         <a:font script="Thai" typeface="Tahoma"/>
@@ -159,10 +159,10 @@
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¯ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¼ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ­ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¯ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¼ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ³ ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¯ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¼ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ°ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ£ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ´ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ£ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ·ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ£ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ£ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¯"/>
-        <a:font script="Hang" typeface="ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ«ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ§ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¬ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂªÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ³ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ«ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ"/>
-        <a:font script="Hans" typeface="ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¥ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ®ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¤ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ½ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ"/>
-        <a:font script="Hant" typeface="ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¦ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ°ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ§ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ´ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ°ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¦ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ©ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ«ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ"/>
+        <a:font script="Jpan" typeface="ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¯ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¼ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ­ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¯ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¼ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ³ ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¯ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¼ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ°ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ£ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ´ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ£ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ·ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ£ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ£ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¯"/>
+        <a:font script="Hang" typeface="ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ«ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ§ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¬ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂªÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ³ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ«ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ"/>
+        <a:font script="Hans" typeface="ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¥ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ®ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¤ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ½ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ"/>
+        <a:font script="Hant" typeface="ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¦ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ°ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ§ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ´ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ°ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ¦ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ©ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ«ÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂÃÂ"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
         <a:font script="Thai" typeface="Tahoma"/>

</xml_diff>